<commit_message>
fix last few saving issues, add clearsheet tests
</commit_message>
<xml_diff>
--- a/output/excel/testwrite.xlsx
+++ b/output/excel/testwrite.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anthony.webster\Documents\projects\perchlorates\output\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B04AEF8-5865-44AE-B12B-997AC87368E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B36E3B-AD84-468B-8CAF-34D77B33B9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
     <sheet name="Char" sheetId="5" r:id="rId2"/>
-    <sheet name="Input" sheetId="9" r:id="rId3"/>
+    <sheet name="Input" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -709,7 +709,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4647A1-8ABF-4A08-8EFB-7C0A2D836087}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C950FCC-AD56-41EE-BD8B-868A2EE044E8}">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>